<commit_message>
Add Inflation data (to modify Engel)
</commit_message>
<xml_diff>
--- a/Data/inflation.xlsx
+++ b/Data/inflation.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhash\OneDrive\Documents\GitHub\IRHEIS\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Majid\Documents\GitHub\IRHEIS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB11739-2DA5-463E-8A48-E6A6BD263B4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69143A85-2A7A-4E5F-8CE9-5403125922BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9570" yWindow="4440" windowWidth="7897" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,149 +30,94 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Majid Einian</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{6A6E9341-1FB2-4268-9D4B-238700546451}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Majid Einian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+link:
+https://www.amar.org.ir/%D9%BE%D8%A7%DB%8C%DA%AF%D8%A7%D9%87-%D9%87%D8%A7-%D9%88-%D8%B3%D8%A7%D9%85%D8%A7%D9%86%D9%87-%D9%87%D8%A7/%D8%B3%D8%B1%DB%8C%D9%87%D8%A7%DB%8C-%D8%B2%D9%85%D8%A7%D9%86%DB%8C/agentType/ViewType/PropertyTypeID/2066</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Year</t>
   </si>
   <si>
-    <t>Inflation</t>
+    <t>D2Inf</t>
   </si>
   <si>
-    <t>18.1</t>
-  </si>
-  <si>
-    <t>20.1</t>
-  </si>
-  <si>
-    <t>12.6</t>
-  </si>
-  <si>
-    <t>11.4</t>
-  </si>
-  <si>
-    <t>15.8</t>
-  </si>
-  <si>
-    <t>15.6</t>
-  </si>
-  <si>
-    <t>15.2</t>
-  </si>
-  <si>
-    <t>10.4</t>
-  </si>
-  <si>
-    <t>11.9</t>
-  </si>
-  <si>
-    <t>18.4</t>
-  </si>
-  <si>
-    <t>25.4</t>
-  </si>
-  <si>
-    <t>10.8</t>
-  </si>
-  <si>
-    <t>12.4</t>
-  </si>
-  <si>
-    <t>21.5</t>
-  </si>
-  <si>
-    <t>30.5</t>
-  </si>
-  <si>
-    <t>34.7</t>
-  </si>
-  <si>
-    <t>9.6</t>
-  </si>
-  <si>
-    <t>9.0</t>
-  </si>
-  <si>
-    <t>26.9</t>
-  </si>
-  <si>
-    <t>CPI</t>
-  </si>
-  <si>
-    <t>6.258</t>
-  </si>
-  <si>
-    <t>7.516</t>
-  </si>
-  <si>
-    <t>8.463</t>
-  </si>
-  <si>
-    <t>9.427</t>
-  </si>
-  <si>
-    <t>10.915</t>
-  </si>
-  <si>
-    <t>14.544</t>
-  </si>
-  <si>
-    <t>16.048</t>
-  </si>
-  <si>
-    <t>17.955</t>
-  </si>
-  <si>
-    <t>21.265</t>
-  </si>
-  <si>
-    <t>26.66</t>
-  </si>
-  <si>
-    <t>29.527</t>
-  </si>
-  <si>
-    <t>33.188</t>
-  </si>
-  <si>
-    <t>40.321</t>
-  </si>
-  <si>
-    <t>52.635</t>
-  </si>
-  <si>
-    <t>70.916</t>
-  </si>
-  <si>
-    <t>81.948</t>
-  </si>
-  <si>
-    <t>91.714</t>
-  </si>
-  <si>
-    <t>109.6</t>
-  </si>
-  <si>
-    <t>164.3</t>
+    <t>D2FoodInf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -197,8 +142,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,20 +423,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="9.1328125" customWidth="1"/>
-    <col min="6" max="6" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,243 +443,231 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>77</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>78</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C3" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>79</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C4" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>80</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C5" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>81</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C6" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>82</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C7" s="1">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>83</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C8" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>84</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B9" s="1">
+        <v>0.11699999999999999</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>85</v>
       </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B10" s="1">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>86</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B11" s="1">
+        <v>0.191</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.18333333333333335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>87</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B12" s="1">
+        <v>0.252</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.25352112676056326</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>88</v>
       </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B13" s="1">
+        <v>0.109</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.10486891385767794</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>89</v>
       </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B14" s="1">
+        <v>0.13699999999999998</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.12542372881355934</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>90</v>
       </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B15" s="1">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.21385542168674676</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>91</v>
       </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B16" s="1">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.30521091811414403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>92</v>
       </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B17" s="1">
+        <v>0.315</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.34790874524714832</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>93</v>
       </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B18" s="1">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.155148095909732</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>94</v>
       </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B19" s="1">
+        <v>0.11900000000000001</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.11965811965811968</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>95</v>
       </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B20" s="1">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>9.0512540894220228E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>96</v>
       </c>
-      <c r="B21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B21" s="2">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>97</v>
       </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" t="s">
-        <v>40</v>
+      <c r="B22" s="2">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="13.9" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>98</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.40200000000000002</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add 99 inflation info.
</commit_message>
<xml_diff>
--- a/Data/inflation.xlsx
+++ b/Data/inflation.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhash\OneDrive\Documents\GitHub\IRHEIS\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Majid\Documents\GitHub\IRHEIS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91280E8E-845A-4458-984D-61DC84C44BC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15060" yWindow="1635" windowWidth="10260" windowHeight="7560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16065" yWindow="1635" windowWidth="10260" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Majid Einian</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{6A6E9341-1FB2-4268-9D4B-238700546451}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -85,13 +84,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -99,7 +98,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -420,19 +419,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.1328125" customWidth="1"/>
+    <col min="2" max="2" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,12 +445,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>78</v>
       </c>
@@ -459,7 +458,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>79</v>
       </c>
@@ -467,7 +466,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>80</v>
       </c>
@@ -475,7 +474,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>81</v>
       </c>
@@ -483,7 +482,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>82</v>
       </c>
@@ -491,7 +490,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>83</v>
       </c>
@@ -502,7 +501,7 @@
         <v>14.544</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>84</v>
       </c>
@@ -516,7 +515,7 @@
         <v>16.047999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>85</v>
       </c>
@@ -530,7 +529,7 @@
         <v>17.954999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>86</v>
       </c>
@@ -544,7 +543,7 @@
         <v>21.265000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>87</v>
       </c>
@@ -558,7 +557,7 @@
         <v>26.66</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>88</v>
       </c>
@@ -572,7 +571,7 @@
         <v>29.527000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>89</v>
       </c>
@@ -586,7 +585,7 @@
         <v>33.188000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>90</v>
       </c>
@@ -600,7 +599,7 @@
         <v>40.320999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>91</v>
       </c>
@@ -614,7 +613,7 @@
         <v>52.634999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>92</v>
       </c>
@@ -628,7 +627,7 @@
         <v>70.914000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>93</v>
       </c>
@@ -642,7 +641,7 @@
         <v>81.947999999999993</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>94</v>
       </c>
@@ -656,7 +655,7 @@
         <v>91.713999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>95</v>
       </c>
@@ -670,7 +669,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>96</v>
       </c>
@@ -684,7 +683,7 @@
         <v>109.65</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>97</v>
       </c>
@@ -698,7 +697,7 @@
         <v>143.84200000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" ht="13.9" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>98</v>
       </c>
@@ -710,6 +709,20 @@
       </c>
       <c r="D23">
         <v>203.15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="13.9" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>99</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="D24">
+        <v>252.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PovertyLine Prediction Update + Some Edits
</commit_message>
<xml_diff>
--- a/Data/inflation.xlsx
+++ b/Data/inflation.xlsx
@@ -1,24 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhash\OneDrive\Documents\GitHub\IRHEIS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91280E8E-845A-4458-984D-61DC84C44BC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45088783-7070-4B0D-9FEE-ED4EDF6D1E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15060" yWindow="1635" windowWidth="10260" windowHeight="7560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -30,7 +40,42 @@
     <author>Majid Einian</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{6A6E9341-1FB2-4268-9D4B-238700546451}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{AD93C3AA-1087-4BE6-8CDD-7CC81E7257F2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Majid Einian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+link:
+https://www.amar.org.ir/%D9%BE%D8%A7%DB%8C%DA%AF%D8%A7%D9%87-%D9%87%D8%A7-%D9%88-%D8%B3%D8%A7%D9%85%D8%A7%D9%86%D9%87-%D9%87%D8%A7/%D8%B3%D8%B1%DB%8C%D9%87%D8%A7%DB%8C-%D8%B2%D9%85%D8%A7%D9%86%DB%8C/agentType/ViewType/PropertyTypeID/2066</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Majid Einian</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{E2D9D02E-7F56-412B-B8E0-A17BE4878E00}">
       <text>
         <r>
           <rPr>
@@ -60,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Year</t>
   </si>
@@ -73,15 +118,34 @@
   <si>
     <t>CPI</t>
   </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>HouseInf</t>
+  </si>
+  <si>
+    <t>AmusementInf</t>
+  </si>
+  <si>
+    <t>HygineInf</t>
+  </si>
+  <si>
+    <t>EduInf</t>
+  </si>
+  <si>
+    <t>FoodInf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +180,17 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -125,7 +200,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -133,14 +208,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,295 +548,481 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView rightToLeft="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="9.1328125" customWidth="1"/>
+    <col min="7" max="7" width="14.53125" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>78</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>0.22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>79</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>0.09</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>80</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>81</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>0.19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>82</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>0.16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>83</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>14.544</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>84</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C9" s="1">
         <v>0.11699999999999999</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>0.11</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>16.047999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>85</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1">
         <v>0.13700000000000001</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>0.13</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>17.954999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>86</v>
       </c>
-      <c r="B11" s="1">
+      <c r="C11" s="1">
         <v>0.191</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>0.18333333333333335</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>21.265000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>87</v>
       </c>
-      <c r="B12" s="1">
+      <c r="C12" s="1">
         <v>0.252</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>0.25352112676056326</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>26.66</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>88</v>
       </c>
-      <c r="B13" s="1">
+      <c r="C13" s="1">
         <v>0.109</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>0.10486891385767794</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>29.527000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>89</v>
       </c>
-      <c r="B14" s="1">
+      <c r="C14" s="1">
         <v>0.13699999999999998</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>0.12542372881355934</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>33.188000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>90</v>
       </c>
-      <c r="B15" s="1">
+      <c r="C15" s="1">
         <v>0.25600000000000001</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>0.21385542168674676</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>40.320999999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F15" s="3">
+        <v>51.377048905602365</v>
+      </c>
+      <c r="G15" s="3">
+        <v>39.855979803341619</v>
+      </c>
+      <c r="H15" s="3">
+        <v>38.788929441366122</v>
+      </c>
+      <c r="I15" s="3">
+        <v>52.185240470517371</v>
+      </c>
+      <c r="J15" s="3">
+        <v>37.179514810692829</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>91</v>
       </c>
-      <c r="B16" s="1">
+      <c r="C16" s="1">
         <v>0.27100000000000002</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>0.30521091811414403</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>52.634999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F16" s="3">
+        <v>60.378633979629505</v>
+      </c>
+      <c r="G16" s="3">
+        <v>53.162034827225519</v>
+      </c>
+      <c r="H16" s="3">
+        <v>47.152090440311824</v>
+      </c>
+      <c r="I16" s="3">
+        <v>57.475530084875878</v>
+      </c>
+      <c r="J16" s="3">
+        <v>53.847622194667359</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>92</v>
       </c>
-      <c r="B17" s="1">
+      <c r="C17" s="1">
         <v>0.315</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>0.34790874524714832</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>70.914000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F17" s="3">
+        <v>73.361618028051922</v>
+      </c>
+      <c r="G17" s="3">
+        <v>74.27423706790772</v>
+      </c>
+      <c r="H17" s="3">
+        <v>65.715537508049209</v>
+      </c>
+      <c r="I17" s="3">
+        <v>65.113133151624922</v>
+      </c>
+      <c r="J17" s="3">
+        <v>77.345466702905</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>93</v>
       </c>
-      <c r="B18" s="1">
+      <c r="C18" s="1">
         <v>0.14599999999999999</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>0.155148095909732</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>81.947999999999993</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F18" s="3">
+        <v>85.74952762109244</v>
+      </c>
+      <c r="G18" s="3">
+        <v>85.499460296099016</v>
+      </c>
+      <c r="H18" s="3">
+        <v>79.483223427826189</v>
+      </c>
+      <c r="I18" s="3">
+        <v>75.936225401496912</v>
+      </c>
+      <c r="J18" s="3">
+        <v>84.800153603268669</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>94</v>
       </c>
-      <c r="B19" s="1">
+      <c r="C19" s="1">
         <v>0.11900000000000001</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D19" s="1">
         <v>0.11965811965811968</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>91.713999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F19" s="3">
+        <v>95.378302947854806</v>
+      </c>
+      <c r="G19" s="3">
+        <v>94.917592000627948</v>
+      </c>
+      <c r="H19" s="3">
+        <v>91.541322754370739</v>
+      </c>
+      <c r="I19" s="3">
+        <v>88.524627202200477</v>
+      </c>
+      <c r="J19" s="3">
+        <v>93.141109733898119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>95</v>
       </c>
-      <c r="B20" s="1">
+      <c r="C20" s="1">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>9.0512540894220228E-2</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F20" s="4">
+        <v>100</v>
+      </c>
+      <c r="G20" s="4">
+        <v>99.999999999999972</v>
+      </c>
+      <c r="H20" s="4">
+        <v>100</v>
+      </c>
+      <c r="I20" s="4">
+        <v>100.00000000000003</v>
+      </c>
+      <c r="J20" s="4">
+        <v>100.00000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>96</v>
       </c>
-      <c r="B21" s="2">
+      <c r="C21" s="2">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="C21" s="2">
+      <c r="D21" s="2">
         <v>0.115</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>109.65</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F21" s="5">
+        <v>106.90748396765704</v>
+      </c>
+      <c r="G21" s="5">
+        <v>107.50507522640768</v>
+      </c>
+      <c r="H21" s="5">
+        <v>107.20563981699416</v>
+      </c>
+      <c r="I21" s="5">
+        <v>111.30793880581165</v>
+      </c>
+      <c r="J21" s="5">
+        <v>112.28134336344182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>97</v>
       </c>
-      <c r="B22" s="2">
+      <c r="C22" s="2">
         <v>0.26900000000000002</v>
       </c>
-      <c r="C22" s="2">
+      <c r="D22" s="2">
         <v>0.36499999999999999</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>143.84200000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F22" s="5">
+        <v>126.6575736080608</v>
+      </c>
+      <c r="G22" s="5">
+        <v>154.29380108548122</v>
+      </c>
+      <c r="H22" s="5">
+        <v>125.60413538447612</v>
+      </c>
+      <c r="I22" s="5">
+        <v>130.80187745110319</v>
+      </c>
+      <c r="J22" s="5">
+        <v>153.60344826838451</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>98</v>
       </c>
-      <c r="B23" s="2">
+      <c r="C23" s="2">
         <v>0.34599999999999997</v>
       </c>
-      <c r="C23" s="2">
+      <c r="D23" s="2">
         <v>0.40200000000000002</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>203.15</v>
+      </c>
+      <c r="F23" s="5">
+        <v>155.71354187966131</v>
+      </c>
+      <c r="G23" s="5">
+        <v>224.5181061339153</v>
+      </c>
+      <c r="H23" s="5">
+        <v>158.13934480472997</v>
+      </c>
+      <c r="I23" s="5">
+        <v>159.34693107134098</v>
+      </c>
+      <c r="J23" s="5">
+        <v>219.65769263128783</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>99</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="E24">
+        <v>252.6</v>
+      </c>
+      <c r="F24" s="5">
+        <v>198.11495099821195</v>
+      </c>
+      <c r="G24" s="5">
+        <v>319.88134178578099</v>
+      </c>
+      <c r="H24" s="5">
+        <v>205.3510871556276</v>
+      </c>
+      <c r="I24" s="5">
+        <v>193.67614465533242</v>
+      </c>
+      <c r="J24" s="5">
+        <v>305.4889571972621</v>
       </c>
     </row>
   </sheetData>
@@ -718,4 +1031,714 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA9D6EB-0266-4A30-8D6D-0FD4EC0FD285}">
+  <dimension ref="A1:E47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>78</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>79</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>80</v>
+      </c>
+      <c r="D5" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>81</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>82</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>83</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E8">
+        <v>14.544</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>84</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.11699999999999999</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="E9">
+        <v>16.047999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>85</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="E10">
+        <v>17.954999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>86</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.191</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.18333333333333335</v>
+      </c>
+      <c r="E11">
+        <v>21.265000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>87</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.252</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.25352112676056326</v>
+      </c>
+      <c r="E12">
+        <v>26.66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>88</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.109</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.10486891385767794</v>
+      </c>
+      <c r="E13">
+        <v>29.527000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>89</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.13699999999999998</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.12542372881355934</v>
+      </c>
+      <c r="E14">
+        <v>33.188000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>90</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.21385542168674676</v>
+      </c>
+      <c r="E15">
+        <v>40.320999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>91</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.30521091811414403</v>
+      </c>
+      <c r="E16">
+        <v>52.634999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>92</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.315</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.34790874524714832</v>
+      </c>
+      <c r="E17">
+        <v>70.914000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>93</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.155148095909732</v>
+      </c>
+      <c r="E18">
+        <v>81.947999999999993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>94</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.11900000000000001</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.11965811965811968</v>
+      </c>
+      <c r="E19">
+        <v>91.713999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>95</v>
+      </c>
+      <c r="C20" s="1">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>9.0512540894220228E-2</v>
+      </c>
+      <c r="E20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>96</v>
+      </c>
+      <c r="C21" s="2">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.115</v>
+      </c>
+      <c r="E21">
+        <v>109.65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>97</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="E22">
+        <v>143.84200000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>98</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="E23">
+        <v>203.15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>98</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.31004628453831456</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.42901292669201863</v>
+      </c>
+      <c r="E24">
+        <v>170.89543746572323</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>98</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.3484853570909911</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.48830509923006987</v>
+      </c>
+      <c r="E25">
+        <v>173.49845634206136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>98</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.38293356883329638</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.53696517364142549</v>
+      </c>
+      <c r="E26">
+        <v>174.85206363675752</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>98</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.41274239203349194</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.58017986187977444</v>
+      </c>
+      <c r="E27">
+        <v>179.66161783349469</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>98</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.43070136363155798</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.60035700863145391</v>
+      </c>
+      <c r="E28">
+        <v>180.82464726616655</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>98</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.43731419715176484</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.60042396758874328</v>
+      </c>
+      <c r="E29">
+        <v>181.73249353897614</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>98</v>
+      </c>
+      <c r="B30">
+        <v>7</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.42845027105153122</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.57543222648701908</v>
+      </c>
+      <c r="E30">
+        <v>184.89994653268678</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>98</v>
+      </c>
+      <c r="B31">
+        <v>8</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.41710071650956621</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.54760834754067078</v>
+      </c>
+      <c r="E31">
+        <v>187.7912951478279</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>98</v>
+      </c>
+      <c r="B32">
+        <v>9</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.40511121252680593</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.5200429413532297</v>
+      </c>
+      <c r="E32">
+        <v>193.78049466904352</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>98</v>
+      </c>
+      <c r="B33">
+        <v>10</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.38962838971463382</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.48778113472074125</v>
+      </c>
+      <c r="E33">
+        <v>195.42278926243088</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>98</v>
+      </c>
+      <c r="B34">
+        <v>11</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.3704568673908426</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.44950946483429388</v>
+      </c>
+      <c r="E34">
+        <v>197.58214004318305</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>98</v>
+      </c>
+      <c r="B35">
+        <v>12</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.34558857332106696</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.40197119495828559</v>
+      </c>
+      <c r="E35">
+        <v>200.47008169607716</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>99</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="E36">
+        <v>252.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>99</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>0.31476961467584319</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.34453829435975453</v>
+      </c>
+      <c r="E37">
+        <v>204.78012901375573</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>99</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>0.28732197539623883</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.29598769332658376</v>
+      </c>
+      <c r="E38">
+        <v>209.97439062431474</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>99</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>0.26473084772188371</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.25853368274172056</v>
+      </c>
+      <c r="E39">
+        <v>214.16144381413679</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>99</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>0.24886751594650108</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.23242919937430301</v>
+      </c>
+      <c r="E40">
+        <v>227.9154559944113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>99</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>0.24103742079595761</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.21985255334276019</v>
+      </c>
+      <c r="E41">
+        <v>235.85144274635934</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>99</v>
+      </c>
+      <c r="B42">
+        <v>6</v>
+      </c>
+      <c r="C42">
+        <v>0.24017605573273015</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.21912928463794018</v>
+      </c>
+      <c r="E42">
+        <v>244.31895592710285</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>99</v>
+      </c>
+      <c r="B43">
+        <v>7</v>
+      </c>
+      <c r="C43">
+        <v>0.25011678485425565</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.2347540707685529</v>
+      </c>
+      <c r="E43">
+        <v>261.52621262125109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>99</v>
+      </c>
+      <c r="B44">
+        <v>8</v>
+      </c>
+      <c r="C44">
+        <v>0.2679830488186204</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.26576712917602352</v>
+      </c>
+      <c r="E44">
+        <v>274.9998954792772</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>99</v>
+      </c>
+      <c r="B45">
+        <v>9</v>
+      </c>
+      <c r="C45">
+        <v>0.28449429697591055</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="E45">
+        <v>280.55000987995913</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>99</v>
+      </c>
+      <c r="B46">
+        <v>10</v>
+      </c>
+      <c r="C46">
+        <v>0.30340859999999997</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="E46">
+        <v>285.67403567764165</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>99</v>
+      </c>
+      <c r="B47">
+        <v>11</v>
+      </c>
+      <c r="C47">
+        <v>0.32662400000000003</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="E47">
+        <v>292.81795885716025</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revised Based on data year 1400
</commit_message>
<xml_diff>
--- a/Data/inflation.xlsx
+++ b/Data/inflation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Majid\Documents\GitHub\IRHEIS\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Refah Economy\IRHEIS-master update 28-8-2022\IRHEIS-master\IRHEIS-master\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07BF675-66FA-49AA-BEF2-F6AD5907722A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B71F79E-F4EA-4ABA-B6E1-EBBC60683E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2512" yWindow="0" windowWidth="11416" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -140,13 +140,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -154,7 +154,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -539,19 +539,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:D24"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="11.3125" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -580,12 +580,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>78</v>
       </c>
@@ -593,7 +593,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>79</v>
       </c>
@@ -601,7 +601,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>80</v>
       </c>
@@ -609,7 +609,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>81</v>
       </c>
@@ -617,7 +617,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>82</v>
       </c>
@@ -625,7 +625,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>83</v>
       </c>
@@ -636,7 +636,7 @@
         <v>14.544</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>84</v>
       </c>
@@ -650,7 +650,7 @@
         <v>16.047999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>85</v>
       </c>
@@ -664,7 +664,7 @@
         <v>17.954999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>86</v>
       </c>
@@ -678,7 +678,7 @@
         <v>21.265000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>87</v>
       </c>
@@ -692,7 +692,7 @@
         <v>26.66</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>88</v>
       </c>
@@ -706,7 +706,7 @@
         <v>29.527000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>89</v>
       </c>
@@ -720,7 +720,7 @@
         <v>33.188000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>90</v>
       </c>
@@ -749,7 +749,7 @@
         <v>37.179514810692829</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>91</v>
       </c>
@@ -778,7 +778,7 @@
         <v>53.847622194667359</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>92</v>
       </c>
@@ -807,7 +807,7 @@
         <v>77.345466702905</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>93</v>
       </c>
@@ -836,7 +836,7 @@
         <v>84.800153603268669</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>94</v>
       </c>
@@ -865,7 +865,7 @@
         <v>93.141109733898119</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>95</v>
       </c>
@@ -894,7 +894,7 @@
         <v>100.00000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>96</v>
       </c>
@@ -923,7 +923,7 @@
         <v>112.28134336344182</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>97</v>
       </c>
@@ -952,7 +952,7 @@
         <v>153.60344826838451</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>98</v>
       </c>
@@ -981,7 +981,7 @@
         <v>219.65769263128783</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>99</v>
       </c>
@@ -1008,6 +1008,20 @@
       </c>
       <c r="I24" s="5">
         <v>305.4889571972621</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>100</v>
+      </c>
+      <c r="B25">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="C25">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="D25">
+        <v>354.1</v>
       </c>
     </row>
   </sheetData>
@@ -1026,9 +1040,9 @@
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1045,12 +1059,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>78</v>
       </c>
@@ -1058,7 +1072,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>79</v>
       </c>
@@ -1066,7 +1080,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>80</v>
       </c>
@@ -1074,7 +1088,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>81</v>
       </c>
@@ -1082,7 +1096,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>82</v>
       </c>
@@ -1090,7 +1104,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>83</v>
       </c>
@@ -1101,7 +1115,7 @@
         <v>14.544</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>84</v>
       </c>
@@ -1115,7 +1129,7 @@
         <v>16.047999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>85</v>
       </c>
@@ -1129,7 +1143,7 @@
         <v>17.954999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>86</v>
       </c>
@@ -1143,7 +1157,7 @@
         <v>21.265000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>87</v>
       </c>
@@ -1157,7 +1171,7 @@
         <v>26.66</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>88</v>
       </c>
@@ -1171,7 +1185,7 @@
         <v>29.527000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>89</v>
       </c>
@@ -1185,7 +1199,7 @@
         <v>33.188000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>90</v>
       </c>
@@ -1199,7 +1213,7 @@
         <v>40.320999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>91</v>
       </c>
@@ -1213,7 +1227,7 @@
         <v>52.634999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>92</v>
       </c>
@@ -1227,7 +1241,7 @@
         <v>70.914000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>93</v>
       </c>
@@ -1241,7 +1255,7 @@
         <v>81.947999999999993</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>94</v>
       </c>
@@ -1255,7 +1269,7 @@
         <v>91.713999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>95</v>
       </c>
@@ -1269,7 +1283,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>96</v>
       </c>
@@ -1283,7 +1297,7 @@
         <v>109.65</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>97</v>
       </c>
@@ -1297,7 +1311,7 @@
         <v>143.84200000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>98</v>
       </c>
@@ -1314,7 +1328,7 @@
         <v>203.15</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>98</v>
       </c>
@@ -1331,7 +1345,7 @@
         <v>170.89543746572323</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>98</v>
       </c>
@@ -1348,7 +1362,7 @@
         <v>173.49845634206136</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>98</v>
       </c>
@@ -1365,7 +1379,7 @@
         <v>174.85206363675752</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>98</v>
       </c>
@@ -1382,7 +1396,7 @@
         <v>179.66161783349469</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>98</v>
       </c>
@@ -1399,7 +1413,7 @@
         <v>180.82464726616655</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>98</v>
       </c>
@@ -1416,7 +1430,7 @@
         <v>181.73249353897614</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>98</v>
       </c>
@@ -1433,7 +1447,7 @@
         <v>184.89994653268678</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>98</v>
       </c>
@@ -1450,7 +1464,7 @@
         <v>187.7912951478279</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>98</v>
       </c>
@@ -1467,7 +1481,7 @@
         <v>193.78049466904352</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>98</v>
       </c>
@@ -1484,7 +1498,7 @@
         <v>195.42278926243088</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>98</v>
       </c>
@@ -1501,7 +1515,7 @@
         <v>197.58214004318305</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>98</v>
       </c>
@@ -1518,7 +1532,7 @@
         <v>200.47008169607716</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>99</v>
       </c>
@@ -1535,7 +1549,7 @@
         <v>252.6</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>99</v>
       </c>
@@ -1552,7 +1566,7 @@
         <v>204.78012901375573</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>99</v>
       </c>
@@ -1569,7 +1583,7 @@
         <v>209.97439062431474</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>99</v>
       </c>
@@ -1586,7 +1600,7 @@
         <v>214.16144381413679</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>99</v>
       </c>
@@ -1603,7 +1617,7 @@
         <v>227.9154559944113</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>99</v>
       </c>
@@ -1620,7 +1634,7 @@
         <v>235.85144274635934</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>99</v>
       </c>
@@ -1637,7 +1651,7 @@
         <v>244.31895592710285</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>99</v>
       </c>
@@ -1654,7 +1668,7 @@
         <v>261.52621262125109</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>99</v>
       </c>
@@ -1671,7 +1685,7 @@
         <v>274.9998954792772</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>99</v>
       </c>
@@ -1688,7 +1702,7 @@
         <v>280.55000987995913</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>99</v>
       </c>
@@ -1705,7 +1719,7 @@
         <v>285.67403567764165</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>99</v>
       </c>
@@ -1722,7 +1736,7 @@
         <v>292.81795885716025</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>99</v>
       </c>
@@ -1733,7 +1747,7 @@
         <v>0.35245903121811401</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>100</v>
       </c>
@@ -1741,7 +1755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>100</v>
       </c>
@@ -1752,7 +1766,7 @@
         <v>0.38089376294181193</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>100</v>
       </c>
@@ -1763,7 +1777,7 @@
         <v>0.40715669106296642</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>100</v>
       </c>
@@ -1774,7 +1788,7 @@
         <v>0.43236598045231461</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>100</v>
       </c>
@@ -1785,7 +1799,7 @@
         <v>0.4490751799720567</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>100</v>
       </c>
@@ -1796,7 +1810,7 @@
         <v>0.46271539051917132</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>100</v>
       </c>
@@ -1807,7 +1821,7 @@
         <v>0.47510601360991928</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>100</v>
       </c>
@@ -1818,7 +1832,7 @@
         <v>0.48006027501524867</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>100</v>
       </c>
@@ -1829,7 +1843,7 @@
         <v>0.47171774394284455</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>100</v>
       </c>
@@ -1840,7 +1854,7 @@
         <v>0.46183957028826428</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>100</v>
       </c>
@@ -1851,7 +1865,7 @@
         <v>0.45190166214418781</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>100</v>
       </c>
@@ -1859,7 +1873,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>100</v>
       </c>

</xml_diff>